<commit_message>
add a summary table
</commit_message>
<xml_diff>
--- a/Numbers-2023/external/CPUresources-2021-2022-2023.xlsx
+++ b/Numbers-2023/external/CPUresources-2021-2022-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schellma/Dropbox/DUNE-computing/CCB-data/Numbers-2023/external/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1070EFF0-0C45-E548-B63B-751E9CF1B4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20626520-6188-0F45-A36E-8F5990142DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="3180" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPUresources-2021-2022-2023" sheetId="1" r:id="rId1"/>
@@ -952,7 +952,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1213,7 +1213,10 @@
         <f t="shared" si="0"/>
         <v>2075</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1">
+        <f>F20-F16-F17</f>
+        <v>6382.5</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1231,7 +1234,10 @@
       <c r="E16" s="1">
         <v>298</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1">
+        <f>F17</f>
+        <v>3191.25</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">

</xml_diff>